<commit_message>
excel is working on mac now
using xlwings version 0.29.0
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57B4F64-7543-E244-8EDE-EB633E6B0B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88EFEE51-42DF-DC44-8B90-4FCFD30A6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{0F06FAC7-0718-9B4D-A8E4-6FF131971962}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{95013AAE-E41E-BA4E-A8D6-6ECC63FE2209}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,6 +35,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>PUMP:HRD:100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details regarding the rechargeable Lithium Polymer Battery. </t>
+  </si>
+  <si>
+    <t>PUMP:HRD:105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details regarding the fuel gauge hardware for the lithium polymer battery. The battery charge shall be displayed to the user. </t>
+  </si>
+  <si>
+    <t>PUMP:HRD:1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details regarding the pressure sensors for use in conjunction with the ideal gas law. </t>
+  </si>
+  <si>
+    <t>PUMP:HRD:3330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details regarding the size and weight of the pump. </t>
+  </si>
+  <si>
+    <t>PUMP:HRD:3350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details regarding the full color touchscreen. </t>
+  </si>
+  <si>
+    <t>Child Tag</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>[PUMP:HRS:100]</t>
+  </si>
+  <si>
+    <t>[PUMP:HRS:103]</t>
+  </si>
+  <si>
+    <t>[PUMP:HRS:1000]</t>
+  </si>
+  <si>
+    <t>[PUMP:HRS:3330]</t>
+  </si>
+  <si>
+    <t>[PUMP:HRS:3350]</t>
+  </si>
+  <si>
+    <t>Parent Tag</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -46,12 +108,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +152,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,13 +471,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FDF735-E74F-4F4D-B744-E0747ACF3697}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D46E14B-C588-9C4A-8D07-672C4228AFFA}">
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected the debugger method
logging library preferred
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88EFEE51-42DF-DC44-8B90-4FCFD30A6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83C9B811-E725-A345-910C-350EC655F3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{95013AAE-E41E-BA4E-A8D6-6ECC63FE2209}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{D49D7BF1-61B7-4042-BF13-E4790D60B83B}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,60 +36,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Report</t>
   </si>
   <si>
-    <t>PUMP:HRD:100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details regarding the rechargeable Lithium Polymer Battery. </t>
-  </si>
-  <si>
-    <t>PUMP:HRD:105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details regarding the fuel gauge hardware for the lithium polymer battery. The battery charge shall be displayed to the user. </t>
-  </si>
-  <si>
-    <t>PUMP:HRD:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details regarding the pressure sensors for use in conjunction with the ideal gas law. </t>
-  </si>
-  <si>
-    <t>PUMP:HRD:3330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details regarding the size and weight of the pump. </t>
-  </si>
-  <si>
-    <t>PUMP:HRD:3350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details regarding the full color touchscreen. </t>
+    <t>PUmp:RISK:10</t>
+  </si>
+  <si>
+    <t>The pump shall deliver no bolus larger than 25 units.</t>
+  </si>
+  <si>
+    <t>pUMP:risk:20</t>
+  </si>
+  <si>
+    <t>The pump shall deliver no basal rate larger than 15 units/hr.</t>
+  </si>
+  <si>
+    <t>PuMP:risk:30</t>
+  </si>
+  <si>
+    <t>The bolus calculator shall provide reverse correction.</t>
+  </si>
+  <si>
+    <t>pump:RISK:40</t>
+  </si>
+  <si>
+    <t>The pump shall display remaining battery charge.</t>
+  </si>
+  <si>
+    <t>PUMp:RISK:50</t>
+  </si>
+  <si>
+    <t>The pump shall display remaining insulin volume.</t>
   </si>
   <si>
     <t>Child Tag</t>
   </si>
   <si>
     <t>Text</t>
-  </si>
-  <si>
-    <t>[PUMP:HRS:100]</t>
-  </si>
-  <si>
-    <t>[PUMP:HRS:103]</t>
-  </si>
-  <si>
-    <t>[PUMP:HRS:1000]</t>
-  </si>
-  <si>
-    <t>[PUMP:HRS:3330]</t>
-  </si>
-  <si>
-    <t>[PUMP:HRS:3350]</t>
   </si>
   <si>
     <t>Parent Tag</t>
@@ -471,7 +456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D46E14B-C588-9C4A-8D07-672C4228AFFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017881C5-BDBD-AB44-82AA-3B2C3F17935D}">
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -479,11 +464,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="106.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -520,7 +505,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -539,9 +524,6 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -559,9 +541,6 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -579,9 +558,6 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -599,9 +575,6 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -618,9 +591,6 @@
       </c>
       <c r="E8" t="s">
         <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
txt file works on mac as well
push commit
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45087A80-2D7F-DD44-84C2-DD9D85FDBC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C0D86A3-21E7-CB45-8297-4446A3B9B99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{73F417CC-D1BC-0442-8F61-8722C9800778}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3421BFFC-61E0-6241-93B3-F86B851E2154}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,45 +36,273 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>Report</t>
   </si>
   <si>
-    <t>PUMP:RISK:10</t>
+    <t>PUMP;RISK;10;</t>
   </si>
   <si>
     <t>The pump shall deliver no bolus larger than 25 units.</t>
   </si>
   <si>
-    <t>PUMP:RISK:20</t>
+    <t>PUMP;RISK;20;</t>
   </si>
   <si>
     <t>The pump shall deliver no basal rate larger than 15 units/hr.</t>
   </si>
   <si>
-    <t>PUMP:RISK:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The bolus calculator shall provide reverse correction. </t>
-  </si>
-  <si>
-    <t>PUMP:RISK:40</t>
-  </si>
-  <si>
-    <t>The pump shall display remaining battery charge.</t>
-  </si>
-  <si>
-    <t>PUMP:RISK:50</t>
-  </si>
-  <si>
-    <t>The pump shall display remaining insulin volume.</t>
+    <t>PUMP;RISK;30;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The polus calculator shall provide reverse correction. </t>
+  </si>
+  <si>
+    <t>PUMP;RISK;40;</t>
+  </si>
+  <si>
+    <t>The pump shall displa remaining battery charge.</t>
+  </si>
+  <si>
+    <t>PUMP;RISK;50;</t>
+  </si>
+  <si>
+    <t>The pump shall display reaining insulin volume.</t>
+  </si>
+  <si>
+    <t>PUMP;RISK;60:</t>
+  </si>
+  <si>
+    <t>The pump shall provide a reminder alarm to change the infusion set;</t>
+  </si>
+  <si>
+    <t>PUMP;RISK;70:</t>
+  </si>
+  <si>
+    <t>The pump shall have the ability to suspend insulin delivery for up to two hours;</t>
+  </si>
+  <si>
+    <t>PUMP;RISK;80:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pump shall have the ability to store at least 90 days of insulin delivery history; </t>
+  </si>
+  <si>
+    <t>PUMP;RISK;90:</t>
+  </si>
+  <si>
+    <t>The pump shall provide automatic shut-off if the insulin cartridge is empty;</t>
+  </si>
+  <si>
+    <t>PUMP;RISK;100:</t>
+  </si>
+  <si>
+    <t>The pump shall provide detailed insulin delivery reports that can be exported as CSV or PDF.</t>
+  </si>
+  <si>
+    <t>PUM;SDS;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the bolus calculator works ….         </t>
+  </si>
+  <si>
+    <t>PUMP;SS;20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the basal rate works …. </t>
+  </si>
+  <si>
+    <t>PUMP;SDS;30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the PID algorithm works ….     </t>
+  </si>
+  <si>
+    <t>PUMP;SDS;40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the GUI works….  </t>
+  </si>
+  <si>
+    <t>UMP;SDS;50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the remaining insulin estimation works… include lots of math …. </t>
+  </si>
+  <si>
+    <t>PUP;SDS;60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the human languages are swapped around </t>
+  </si>
+  <si>
+    <t>PMP;SDS;70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are details of how the battery estimation works </t>
+  </si>
+  <si>
+    <t>AE;SRS;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a bolus feature which generates boluses in the range of 0.01 to 25 units, which an increment of 0.01 units.  </t>
+  </si>
+  <si>
+    <t>CE;SRS;2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a programmable basal rate feature, with basal rates in the range of 0.001 to 15 units/hour in increments of 0.001 u/hr. </t>
+  </si>
+  <si>
+    <t>ACE;SRS;5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a programmable correction factor feature. The software shall support correction factors in the range of 1:10 to 1:600 u/mg/dL. </t>
+  </si>
+  <si>
+    <t>ACE;SRS;6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a programmable carb ratio feature. The software shall support carb ratios in the range of 1:10 to 1:600 u/g. </t>
+  </si>
+  <si>
+    <t>ACE;RS;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a means for the user to select between English, German, French, Spanish, and Czech. </t>
+  </si>
+  <si>
+    <t>AC;SRS;100</t>
+  </si>
+  <si>
+    <t>The GUI shall indicate percent battery charge. The charge shall be displayed in increments of 1%.</t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a bolus calculator feature. </t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bolus size shall be estimated as the sum of the insulin needed to cover the current meal  and correct down to 110 mg/dL. If the sum is negative, the bolus is aborted. </t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The amount of insulin needed to cover the meal shall be estimated only when the user indicates a meal was consumed. The volume of insulin shall be estimated as the number of carbs divided by the CarbRatio.  </t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The amount of insulin needed to correct glucose levels shall be estimated by the following formula if and only if the glucose is greater than 110:  </t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value of CorrectionBolus shall be set to zero when the glucose is between 80 and 110 mg/dL, inclusive. </t>
+  </si>
+  <si>
+    <t>BOLUS;SRS;12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The amount of insulin needed to correct glucose levels shall be estimated by the following formula if and only if the glucose is less than 80. Please note that in this case, the dose amount is a negative number.  </t>
+  </si>
+  <si>
+    <t>AID;SRS;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dosing algorithm shall include a proportional gain term. The algorithm shall allow proportional gains in the range of 0 to 2.0 in increments of 0.001  </t>
+  </si>
+  <si>
+    <t>AID;SRS;2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dosing algorithm shall include a derivative gain term. The algorithm shall allow derivative gains in the range of 0 to 2.0 in increments of 0.001 </t>
+  </si>
+  <si>
+    <t>AID;SRS;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dosing algorithm shall include an integral gain term. The algorithm shall allow integral gains in the range of 0 to 2.0 in increments of 0.001 </t>
+  </si>
+  <si>
+    <t>AID;SRS;12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dosing algorithm shall include an integrator window to minimize limit-cycling. The window shall be settable at compile time to a range of 0.002 to 0.01 in increments of 0.001  </t>
+  </si>
+  <si>
+    <t>AID;SRS;20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dosing algorithm shall include anti-windup reset protection.  </t>
   </si>
   <si>
     <t>Child Tag</t>
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>[BLUS;SRS;1] [BOLUS;SRS;2] [BOLUS;SRS;5] [BOLUS;SRS;6] [BOLUS;SRS;8] [BOLS;SRS;12] [ACE;SRS;1] [ACE;SRS;5] [ACE;SRS;6]</t>
+  </si>
+  <si>
+    <t>[ACE;SRS;2]</t>
+  </si>
+  <si>
+    <t>[AID;SRS;1] [AID;SRS;2] [AID;SRS;10] [AID;SRS;12] [AID;SRS;20]</t>
+  </si>
+  <si>
+    <t>[AE;SRS;110] [ACE;SRS;120]</t>
+  </si>
+  <si>
+    <t>[ACE;SRS;110]</t>
+  </si>
+  <si>
+    <t>[ACE;SRS;10]</t>
+  </si>
+  <si>
+    <t>[ACE;SRS;100]</t>
+  </si>
+  <si>
+    <t>[PMP;PRS;1] [UMP;TBV;1]</t>
+  </si>
+  <si>
+    <t>[PMP;PRS;1]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;5]</t>
+  </si>
+  <si>
+    <t>[PUM;RS;6]</t>
+  </si>
+  <si>
+    <t>[PUMP;PR;10]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;105]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;1]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;1] [PUMP;PRS;5]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;1] [PUMP;PRS;3]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS:1] [PUMP;PRS;8]</t>
+  </si>
+  <si>
+    <t>[PUMP;PRS;4000] [PUMP;DER;2]</t>
   </si>
   <si>
     <t>Parent Tag</t>
@@ -456,19 +684,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0475B262-BB4D-C043-A812-0ECDF53C7A4C}">
-  <dimension ref="A1:S8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5239474F-A381-8542-BF2C-157311DA854A}">
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="179.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
@@ -496,16 +724,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -591,6 +819,571 @@
       </c>
       <c r="E8" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still testing for Targest2.py orphan report
push commit
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CD852C8-7DDE-3946-B250-0394EF429DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9318FF1-AEBD-D447-A599-E4A0EF088664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{077ACF56-F3FC-0D44-80D2-499CB7CA2374}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{46404EEC-0928-B347-9E19-0D039D07CEBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1311,7 +1311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8BAD14-E746-7446-996C-0DAA796ECEC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20110606-199D-CE4E-8F9B-F49DE524ED80}">
   <dimension ref="A1:S123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
still updating the Targest2.py file
push commit
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9318FF1-AEBD-D447-A599-E4A0EF088664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0F13247-50E6-0643-8346-502DB6203441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{46404EEC-0928-B347-9E19-0D039D07CEBB}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{15BEFD08-88E0-C044-AF23-9732B8DBFE7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1311,7 +1311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20110606-199D-CE4E-8F9B-F49DE524ED80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C64BE-B32D-D942-B153-E67B7F0FC0AE}">
   <dimension ref="A1:S123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
testing the df3 variable
push commit
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/colorTest.New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDB3A875-EAF9-4F4B-B1DF-F4B76F9C7E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E98C037-3579-D144-BB88-C9F8E5E30BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{60DBE40D-E7FB-E742-9EEC-B75800E26DD3}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{C1C9E6A2-6DCD-EB40-B54B-3BB7D238F1B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="310">
   <si>
     <t>Report</t>
   </si>
   <si>
+    <t>PUMP:URS:1</t>
+  </si>
+  <si>
+    <t>The pump shall provide both a bolus and basal feature.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:3</t>
+  </si>
+  <si>
+    <t>The software shall provide a bolus calculator which is supported by programmable correction factors and carb ratios.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The software shall provide a reverse correction feature for the bolus calculator. </t>
+  </si>
+  <si>
+    <t>PUMP:URS:10</t>
+  </si>
+  <si>
+    <t>The software shall provide a means for the user to select between at least five different European human languages.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pump shall include a rechargeable Battery. </t>
+  </si>
+  <si>
+    <t>PUMP:URS:103</t>
+  </si>
+  <si>
+    <t>The pump shall display remaining battery charge.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:1000</t>
+  </si>
+  <si>
+    <t>The pump shall display remaining insulin volume.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:3330</t>
+  </si>
+  <si>
+    <t>The pump shall be small and lightweight.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:3350</t>
+  </si>
+  <si>
+    <t>The pump shall be easy to use.</t>
+  </si>
+  <si>
+    <t>PUMP:URS:4000</t>
+  </si>
+  <si>
+    <t>The pump shall include an automated dosing algorithm.</t>
+  </si>
+  <si>
     <t>PUMP:HRD:100</t>
   </si>
   <si>
@@ -290,15 +350,9 @@
     <t>PUMP:RISK:40</t>
   </si>
   <si>
-    <t>The pump shall display remaining battery charge.</t>
-  </si>
-  <si>
     <t>PUMP:RISK:50</t>
   </si>
   <si>
-    <t>The pump shall display remaining insulin volume.</t>
-  </si>
-  <si>
     <t>PUMP:SDS:10</t>
   </si>
   <si>
@@ -644,58 +698,34 @@
     <t xml:space="preserve">Code Inspection Test for pump_mmm.c,h </t>
   </si>
   <si>
-    <t>PUMP:URS:1</t>
-  </si>
-  <si>
-    <t>The pump shall provide both a bolus and basal feature.</t>
-  </si>
-  <si>
-    <t>PUMP:URS:3</t>
-  </si>
-  <si>
-    <t>The software shall provide a bolus calculator which is supported by programmable correction factors and carb ratios.</t>
-  </si>
-  <si>
-    <t>PUMP:URS:8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The software shall provide a reverse correction feature for the bolus calculator. </t>
-  </si>
-  <si>
-    <t>PUMP:URS:10</t>
-  </si>
-  <si>
-    <t>The software shall provide a means for the user to select between at least five different European human languages.</t>
-  </si>
-  <si>
-    <t>PUMP:URS:100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The pump shall include a rechargeable Battery. </t>
-  </si>
-  <si>
-    <t>PUMP:URS:103</t>
-  </si>
-  <si>
-    <t>PUMP:URS:1000</t>
-  </si>
-  <si>
-    <t>PUMP:URS:3330</t>
-  </si>
-  <si>
-    <t>The pump shall be small and lightweight.</t>
-  </si>
-  <si>
-    <t>PUMP:URS:3350</t>
-  </si>
-  <si>
-    <t>The pump shall be easy to use.</t>
-  </si>
-  <si>
-    <t>PUMP:URS:4000</t>
-  </si>
-  <si>
-    <t>The pump shall include an automated dosing algorithm.</t>
+    <t xml:space="preserve">PUMP:URS:1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:103 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:1000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:3330 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:3350 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUMP:URS:4000 </t>
   </si>
   <si>
     <t>Child Tag</t>
@@ -933,6 +963,9 @@
   </si>
   <si>
     <t>Parent Tag</t>
+  </si>
+  <si>
+    <t>Orphan Tags</t>
   </si>
 </sst>
 </file>
@@ -957,12 +990,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -976,6 +1003,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1311,8 +1344,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031F98C3-B1A3-3048-BC3E-796DEF479183}">
-  <dimension ref="A1:S123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D92BFE-F7EA-C649-9774-211B947013D2}">
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1324,46 +1357,33 @@
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="111.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1379,11 +1399,14 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1399,11 +1422,14 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1419,11 +1445,14 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1439,11 +1468,14 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1459,11 +1491,14 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1479,11 +1514,14 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1499,11 +1537,14 @@
       <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1519,11 +1560,14 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1539,11 +1583,14 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1559,11 +1606,14 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1580,10 +1630,10 @@
         <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1600,10 +1650,10 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1620,7 +1670,7 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1640,7 +1690,7 @@
         <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1660,7 +1710,7 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1680,7 +1730,7 @@
         <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1700,7 +1750,7 @@
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1720,7 +1770,7 @@
         <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1740,7 +1790,7 @@
         <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1760,7 +1810,7 @@
         <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1780,7 +1830,7 @@
         <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1791,7 +1841,7 @@
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D25">
         <v>21</v>
@@ -1800,7 +1850,7 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1808,19 +1858,19 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D26">
         <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1828,19 +1878,19 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1848,19 +1898,19 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1868,19 +1918,19 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D29">
         <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1888,16 +1938,16 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D30">
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
         <v>243</v>
@@ -1908,16 +1958,16 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D31">
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
         <v>244</v>
@@ -1928,16 +1978,16 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
         <v>245</v>
@@ -1948,16 +1998,16 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D33">
         <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
         <v>246</v>
@@ -1968,16 +2018,16 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D34">
         <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
         <v>247</v>
@@ -1988,16 +2038,16 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D35">
         <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
         <v>248</v>
@@ -2008,16 +2058,16 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D36">
         <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
         <v>249</v>
@@ -2028,16 +2078,16 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D37">
         <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
         <v>250</v>
@@ -2048,16 +2098,16 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D38">
         <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F38" t="s">
         <v>251</v>
@@ -2068,19 +2118,19 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D39">
         <v>35</v>
       </c>
       <c r="E39" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2088,19 +2138,19 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D40">
         <v>36</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F40" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2108,19 +2158,19 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D41">
         <v>37</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2128,19 +2178,19 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D42">
         <v>38</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F42" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2148,19 +2198,19 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D43">
         <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2168,19 +2218,19 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D44">
         <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2188,19 +2238,19 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D45">
         <v>41</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2208,19 +2258,19 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D46">
         <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2228,19 +2278,19 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D47">
         <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F47" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2248,19 +2298,19 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D48">
         <v>44</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F48" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2268,16 +2318,19 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D49">
         <v>45</v>
       </c>
       <c r="E49" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="F49" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2285,16 +2338,19 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D50">
         <v>46</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="F50" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2302,16 +2358,19 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D51">
         <v>47</v>
       </c>
       <c r="E51" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="F51" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2319,16 +2378,19 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="D52">
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,16 +2398,19 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D53">
         <v>49</v>
       </c>
       <c r="E53" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="F53" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2353,19 +2418,19 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D54">
         <v>50</v>
       </c>
       <c r="E54" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2373,19 +2438,19 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="D55">
         <v>51</v>
       </c>
       <c r="E55" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F55" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2393,19 +2458,19 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D56">
         <v>52</v>
       </c>
       <c r="E56" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F56" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2413,19 +2478,19 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="D57">
         <v>53</v>
       </c>
       <c r="E57" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F57" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2445,7 +2510,7 @@
         <v>95</v>
       </c>
       <c r="F58" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2464,9 +2529,6 @@
       <c r="E59" t="s">
         <v>97</v>
       </c>
-      <c r="F59" t="s">
-        <v>265</v>
-      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -2484,9 +2546,6 @@
       <c r="E60" t="s">
         <v>99</v>
       </c>
-      <c r="F60" t="s">
-        <v>266</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -2504,9 +2563,6 @@
       <c r="E61" t="s">
         <v>101</v>
       </c>
-      <c r="F61" t="s">
-        <v>267</v>
-      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -2516,16 +2572,13 @@
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>58</v>
       </c>
       <c r="E62" t="s">
         <v>103</v>
-      </c>
-      <c r="F62" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2533,19 +2586,16 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="D63">
         <v>59</v>
       </c>
       <c r="E63" t="s">
-        <v>105</v>
-      </c>
-      <c r="F63" t="s">
-        <v>269</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2553,16 +2603,16 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D64">
         <v>60</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F64" t="s">
         <v>270</v>
@@ -2573,16 +2623,16 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D65">
         <v>61</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F65" t="s">
         <v>271</v>
@@ -2593,16 +2643,16 @@
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D66">
         <v>62</v>
       </c>
       <c r="E66" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F66" t="s">
         <v>272</v>
@@ -2613,19 +2663,19 @@
         <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D67">
         <v>63</v>
       </c>
       <c r="E67" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F67" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2633,19 +2683,19 @@
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D68">
         <v>64</v>
       </c>
       <c r="E68" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F68" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2653,19 +2703,19 @@
         <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D69">
         <v>65</v>
       </c>
       <c r="E69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F69" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2673,19 +2723,19 @@
         <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D70">
         <v>66</v>
       </c>
       <c r="E70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F70" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2693,19 +2743,19 @@
         <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C71" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D71">
         <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F71" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2713,19 +2763,19 @@
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C72" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D72">
         <v>68</v>
       </c>
       <c r="E72" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F72" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2733,19 +2783,19 @@
         <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D73">
         <v>69</v>
       </c>
       <c r="E73" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F73" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2753,19 +2803,19 @@
         <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D74">
         <v>70</v>
       </c>
       <c r="E74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F74" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2773,19 +2823,19 @@
         <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C75" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D75">
         <v>71</v>
       </c>
       <c r="E75" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F75" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2793,19 +2843,19 @@
         <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D76">
         <v>72</v>
       </c>
       <c r="E76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F76" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2813,19 +2863,19 @@
         <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D77">
         <v>73</v>
       </c>
       <c r="E77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F77" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2833,19 +2883,19 @@
         <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D78">
         <v>74</v>
       </c>
       <c r="E78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F78" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2853,19 +2903,19 @@
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C79" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D79">
         <v>75</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F79" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2873,19 +2923,19 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D80">
         <v>76</v>
       </c>
       <c r="E80" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F80" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2893,19 +2943,19 @@
         <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D81">
         <v>77</v>
       </c>
       <c r="E81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F81" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2913,19 +2963,19 @@
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C82" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D82">
         <v>78</v>
       </c>
       <c r="E82" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F82" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2933,19 +2983,19 @@
         <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C83" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="D83">
         <v>79</v>
       </c>
       <c r="E83" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F83" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2953,19 +3003,19 @@
         <v>80</v>
       </c>
       <c r="B84" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84" t="s">
         <v>146</v>
-      </c>
-      <c r="C84" t="s">
-        <v>26</v>
       </c>
       <c r="D84">
         <v>80</v>
       </c>
       <c r="E84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F84" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2976,7 +3026,7 @@
         <v>147</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>148</v>
       </c>
       <c r="D85">
         <v>81</v>
@@ -2985,7 +3035,7 @@
         <v>147</v>
       </c>
       <c r="F85" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2993,19 +3043,19 @@
         <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D86">
         <v>82</v>
       </c>
       <c r="E86" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F86" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -3013,19 +3063,19 @@
         <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
       <c r="D87">
         <v>83</v>
       </c>
       <c r="E87" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F87" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3033,19 +3083,19 @@
         <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C88" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D88">
         <v>84</v>
       </c>
       <c r="E88" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F88" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -3053,19 +3103,19 @@
         <v>85</v>
       </c>
       <c r="B89" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C89" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D89">
         <v>85</v>
       </c>
       <c r="E89" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F89" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -3073,19 +3123,19 @@
         <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C90" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D90">
         <v>86</v>
       </c>
       <c r="E90" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F90" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -3093,19 +3143,19 @@
         <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C91" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D91">
         <v>87</v>
       </c>
       <c r="E91" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F91" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -3113,19 +3163,19 @@
         <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C92" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D92">
         <v>88</v>
       </c>
       <c r="E92" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F92" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -3133,16 +3183,16 @@
         <v>89</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="D93">
         <v>89</v>
       </c>
       <c r="E93" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F93" t="s">
         <v>290</v>
@@ -3153,16 +3203,16 @@
         <v>90</v>
       </c>
       <c r="B94" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C94" t="s">
-        <v>163</v>
+        <v>46</v>
       </c>
       <c r="D94">
         <v>90</v>
       </c>
       <c r="E94" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F94" t="s">
         <v>291</v>
@@ -3173,16 +3223,16 @@
         <v>91</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C95" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="D95">
         <v>91</v>
       </c>
       <c r="E95" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F95" t="s">
         <v>292</v>
@@ -3196,7 +3246,7 @@
         <v>166</v>
       </c>
       <c r="C96" t="s">
-        <v>167</v>
+        <v>50</v>
       </c>
       <c r="D96">
         <v>92</v>
@@ -3213,16 +3263,16 @@
         <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C97" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="D97">
         <v>93</v>
       </c>
       <c r="E97" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F97" t="s">
         <v>294</v>
@@ -3233,16 +3283,16 @@
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C98" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D98">
         <v>94</v>
       </c>
       <c r="E98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F98" t="s">
         <v>295</v>
@@ -3253,16 +3303,16 @@
         <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C99" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D99">
         <v>95</v>
       </c>
       <c r="E99" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F99" t="s">
         <v>296</v>
@@ -3273,16 +3323,16 @@
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C100" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D100">
         <v>96</v>
       </c>
       <c r="E100" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F100" t="s">
         <v>297</v>
@@ -3293,19 +3343,19 @@
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D101">
         <v>97</v>
       </c>
       <c r="E101" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F101" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3313,19 +3363,19 @@
         <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D102">
         <v>98</v>
       </c>
       <c r="E102" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F102" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -3333,19 +3383,19 @@
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D103">
         <v>99</v>
       </c>
       <c r="E103" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F103" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -3353,19 +3403,19 @@
         <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C104" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D104">
         <v>100</v>
       </c>
       <c r="E104" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F104" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -3373,19 +3423,19 @@
         <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D105">
         <v>101</v>
       </c>
       <c r="E105" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F105" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -3393,19 +3443,19 @@
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C106" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D106">
         <v>102</v>
       </c>
       <c r="E106" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F106" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -3413,19 +3463,19 @@
         <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D107">
         <v>103</v>
       </c>
       <c r="E107" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F107" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -3433,19 +3483,19 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C108" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D108">
         <v>104</v>
       </c>
       <c r="E108" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F108" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -3453,19 +3503,19 @@
         <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C109" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D109">
         <v>105</v>
       </c>
       <c r="E109" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F109" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -3473,19 +3523,19 @@
         <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C110" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D110">
         <v>106</v>
       </c>
       <c r="E110" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F110" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -3493,16 +3543,16 @@
         <v>107</v>
       </c>
       <c r="B111" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C111" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D111">
         <v>107</v>
       </c>
       <c r="E111" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F111" t="s">
         <v>295</v>
@@ -3513,16 +3563,16 @@
         <v>108</v>
       </c>
       <c r="B112" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C112" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D112">
         <v>108</v>
       </c>
       <c r="E112" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F112" t="s">
         <v>296</v>
@@ -3533,16 +3583,16 @@
         <v>109</v>
       </c>
       <c r="B113" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C113" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D113">
         <v>109</v>
       </c>
       <c r="E113" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F113" t="s">
         <v>297</v>
@@ -3553,16 +3603,19 @@
         <v>110</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C114" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D114">
         <v>110</v>
       </c>
       <c r="E114" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="F114" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -3570,16 +3623,19 @@
         <v>111</v>
       </c>
       <c r="B115" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C115" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D115">
         <v>111</v>
       </c>
       <c r="E115" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+      <c r="F115" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -3587,16 +3643,19 @@
         <v>112</v>
       </c>
       <c r="B116" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C116" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D116">
         <v>112</v>
       </c>
       <c r="E116" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="F116" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -3604,16 +3663,19 @@
         <v>113</v>
       </c>
       <c r="B117" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C117" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D117">
         <v>113</v>
       </c>
       <c r="E117" t="s">
-        <v>208</v>
+        <v>206</v>
+      </c>
+      <c r="F117" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -3621,16 +3683,19 @@
         <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C118" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D118">
         <v>114</v>
       </c>
       <c r="E118" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="F118" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -3638,16 +3703,19 @@
         <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C119" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="D119">
         <v>115</v>
       </c>
       <c r="E119" t="s">
-        <v>212</v>
+        <v>210</v>
+      </c>
+      <c r="F119" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -3655,16 +3723,19 @@
         <v>116</v>
       </c>
       <c r="B120" t="s">
+        <v>212</v>
+      </c>
+      <c r="C120" t="s">
         <v>213</v>
-      </c>
-      <c r="C120" t="s">
-        <v>86</v>
       </c>
       <c r="D120">
         <v>116</v>
       </c>
       <c r="E120" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="F120" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -3683,6 +3754,9 @@
       <c r="E121" t="s">
         <v>214</v>
       </c>
+      <c r="F121" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
@@ -3700,6 +3774,9 @@
       <c r="E122" t="s">
         <v>216</v>
       </c>
+      <c r="F122" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
@@ -3716,6 +3793,9 @@
       </c>
       <c r="E123" t="s">
         <v>218</v>
+      </c>
+      <c r="F123" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>